<commit_message>
working on transformation of each source
</commit_message>
<xml_diff>
--- a/data/T/byHand/housesSmart.xlsx
+++ b/data/T/byHand/housesSmart.xlsx
@@ -8,25 +8,33 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Reference\housemodel\data\T\byHand\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8BE3031-A886-447D-878A-F7D3C028588E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{015D3940-E10B-44C5-8F72-E89B5DEAE428}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Columns" sheetId="1" r:id="rId1"/>
     <sheet name="Dictionary" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="348" uniqueCount="101">
   <si>
     <t>web-scraper-order</t>
   </si>
@@ -317,9 +325,6 @@
     <t>funcRgxPk</t>
   </si>
   <si>
-    <t>IndexCpy</t>
-  </si>
-  <si>
     <t>Number of Baths</t>
   </si>
   <si>
@@ -362,13 +367,10 @@
     <t>State</t>
   </si>
   <si>
-    <t>Done</t>
-  </si>
-  <si>
-    <t>Pending</t>
-  </si>
-  <si>
     <t>Date</t>
+  </si>
+  <si>
+    <t>idxRow</t>
   </si>
 </sst>
 </file>
@@ -544,7 +546,63 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="10">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -837,8 +895,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P35"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="O21" sqref="O21"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1541,68 +1599,97 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0D0F27B-DE69-4889-8F79-7CACC7421700}">
-  <dimension ref="A1:Q12"/>
+  <dimension ref="A1:Y12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+    <sheetView topLeftCell="F1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="O10" sqref="O10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="19.7109375" style="14" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="22.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15" style="14" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="22.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="19.140625" style="14" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="22.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="15" style="14" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="22.42578125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="18.85546875" style="14" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="22.42578125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15" style="14" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="19.140625" style="14" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="15" style="14" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="18.85546875" style="14" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="18.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="19" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:25" s="19" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="20" t="s">
+        <v>98</v>
+      </c>
+      <c r="B1" s="20" t="s">
         <v>99</v>
-      </c>
-      <c r="B1" s="20" t="s">
-        <v>102</v>
       </c>
       <c r="C1" s="16" t="s">
         <v>17</v>
       </c>
       <c r="D1" s="17"/>
       <c r="E1" s="17"/>
-      <c r="F1" s="16" t="s">
+      <c r="F1" s="20" t="s">
+        <v>98</v>
+      </c>
+      <c r="G1" s="20" t="s">
+        <v>99</v>
+      </c>
+      <c r="H1" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="G1" s="17"/>
-      <c r="H1" s="17"/>
-      <c r="I1" s="16" t="s">
+      <c r="I1" s="17"/>
+      <c r="J1" s="17"/>
+      <c r="K1" s="20" t="s">
+        <v>98</v>
+      </c>
+      <c r="L1" s="20" t="s">
+        <v>99</v>
+      </c>
+      <c r="M1" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="J1" s="17"/>
-      <c r="K1" s="17"/>
-      <c r="L1" s="16" t="s">
+      <c r="N1" s="17"/>
+      <c r="O1" s="17"/>
+      <c r="P1" s="20" t="s">
+        <v>98</v>
+      </c>
+      <c r="Q1" s="20" t="s">
+        <v>99</v>
+      </c>
+      <c r="R1" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="M1" s="17"/>
-      <c r="N1" s="17"/>
-      <c r="O1" s="16" t="s">
+      <c r="S1" s="17"/>
+      <c r="T1" s="17"/>
+      <c r="U1" s="20" t="s">
+        <v>98</v>
+      </c>
+      <c r="V1" s="20" t="s">
+        <v>99</v>
+      </c>
+      <c r="W1" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="P1" s="18"/>
-      <c r="Q1" s="17"/>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>100</v>
+      <c r="X1" s="18"/>
+      <c r="Y1" s="17"/>
+    </row>
+    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A2" t="str">
+        <f>IF(ISBLANK(B2),"Pending","Done")</f>
+        <v>Done</v>
       </c>
       <c r="B2" s="7">
         <v>44021</v>
@@ -1616,545 +1703,820 @@
       <c r="E2" s="8" t="s">
         <v>74</v>
       </c>
-      <c r="F2" s="11" t="s">
+      <c r="F2" t="str">
+        <f>IF(ISBLANK(G2),"Pending","Done")</f>
+        <v>Done</v>
+      </c>
+      <c r="G2" s="7">
+        <v>44021</v>
+      </c>
+      <c r="H2" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="I2" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="H2" s="8" t="s">
+      <c r="J2" s="8" t="s">
         <v>74</v>
       </c>
-      <c r="I2" s="11" t="s">
+      <c r="K2" t="str">
+        <f>IF(ISBLANK(L2),"Pending","Done")</f>
+        <v>Done</v>
+      </c>
+      <c r="L2" s="7">
+        <v>44021</v>
+      </c>
+      <c r="M2" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="N2" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="K2" s="8" t="s">
+      <c r="O2" s="8" t="s">
         <v>74</v>
       </c>
-      <c r="L2" s="11" t="s">
+      <c r="P2" t="str">
+        <f>IF(ISBLANK(Q2),"Pending","Done")</f>
+        <v>Done</v>
+      </c>
+      <c r="Q2" s="7">
+        <v>44021</v>
+      </c>
+      <c r="R2" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="M2" s="1" t="s">
+      <c r="S2" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="N2" s="8" t="s">
+      <c r="T2" s="8" t="s">
         <v>74</v>
       </c>
-      <c r="O2" s="11" t="s">
+      <c r="U2" t="str">
+        <f>IF(ISBLANK(V2),"Pending","Done")</f>
+        <v>Done</v>
+      </c>
+      <c r="V2" s="7">
+        <v>44021</v>
+      </c>
+      <c r="W2" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="P2" s="1" t="s">
+      <c r="X2" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="Q2" s="8" t="s">
+      <c r="Y2" s="8" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>101</v>
+    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A3" t="str">
+        <f t="shared" ref="A3:A11" si="0">IF(ISBLANK(B3),"Pending","Done")</f>
+        <v>Done</v>
+      </c>
+      <c r="B3" s="7">
+        <v>44022</v>
       </c>
       <c r="C3" s="14" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="D3" t="s">
-        <v>30</v>
+        <v>13</v>
       </c>
       <c r="E3" t="s">
-        <v>87</v>
-      </c>
-      <c r="F3" s="14" t="s">
-        <v>3</v>
-      </c>
-      <c r="G3" t="s">
-        <v>30</v>
-      </c>
-      <c r="H3" t="s">
-        <v>87</v>
-      </c>
-      <c r="I3" s="14" t="s">
-        <v>3</v>
+        <v>100</v>
+      </c>
+      <c r="F3" t="str">
+        <f t="shared" ref="F3:F11" si="1">IF(ISBLANK(G3),"Pending","Done")</f>
+        <v>Done</v>
+      </c>
+      <c r="G3" s="7">
+        <v>44022</v>
+      </c>
+      <c r="H3" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="I3" t="s">
+        <v>13</v>
       </c>
       <c r="J3" t="s">
-        <v>30</v>
-      </c>
-      <c r="K3" t="s">
-        <v>87</v>
-      </c>
-      <c r="L3" s="14" t="s">
-        <v>3</v>
-      </c>
-      <c r="M3" t="s">
-        <v>30</v>
+        <v>100</v>
+      </c>
+      <c r="K3" t="str">
+        <f t="shared" ref="K3:K11" si="2">IF(ISBLANK(L3),"Pending","Done")</f>
+        <v>Done</v>
+      </c>
+      <c r="L3" s="7">
+        <v>44022</v>
+      </c>
+      <c r="M3" s="14" t="s">
+        <v>13</v>
       </c>
       <c r="N3" t="s">
-        <v>87</v>
-      </c>
-      <c r="O3" s="14" t="s">
-        <v>3</v>
-      </c>
-      <c r="P3" t="s">
-        <v>30</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>101</v>
-      </c>
-      <c r="C4" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="O3" t="s">
+        <v>100</v>
+      </c>
+      <c r="P3" t="str">
+        <f t="shared" ref="P3:P11" si="3">IF(ISBLANK(Q3),"Pending","Done")</f>
+        <v>Done</v>
+      </c>
+      <c r="Q3" s="7">
+        <v>44022</v>
+      </c>
+      <c r="R3" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="S3" t="s">
+        <v>13</v>
+      </c>
+      <c r="T3" t="s">
+        <v>100</v>
+      </c>
+      <c r="U3" t="str">
+        <f t="shared" ref="U3:U11" si="4">IF(ISBLANK(V3),"Pending","Done")</f>
+        <v>Done</v>
+      </c>
+      <c r="V3" s="7">
+        <v>44022</v>
+      </c>
+      <c r="W3" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="X3" t="s">
+        <v>13</v>
+      </c>
+      <c r="Y3" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A4" t="str">
+        <f t="shared" si="0"/>
+        <v>Pending</v>
+      </c>
+      <c r="C4" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" t="s">
+        <v>90</v>
+      </c>
+      <c r="E4" t="s">
+        <v>86</v>
+      </c>
+      <c r="F4" t="str">
+        <f t="shared" si="1"/>
+        <v>Pending</v>
+      </c>
+      <c r="H4" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="I4" t="s">
+        <v>90</v>
+      </c>
+      <c r="J4" t="s">
+        <v>86</v>
+      </c>
+      <c r="K4" t="str">
+        <f t="shared" si="2"/>
+        <v>Pending</v>
+      </c>
+      <c r="M4" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="N4" t="s">
+        <v>90</v>
+      </c>
+      <c r="O4" t="s">
+        <v>86</v>
+      </c>
+      <c r="P4" t="str">
+        <f t="shared" si="3"/>
+        <v>Pending</v>
+      </c>
+      <c r="R4" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="S4" t="s">
+        <v>90</v>
+      </c>
+      <c r="T4" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="U4" t="str">
+        <f t="shared" si="4"/>
+        <v>Pending</v>
+      </c>
+      <c r="W4" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="X4" t="s">
+        <v>90</v>
+      </c>
+      <c r="Y4" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A5" t="str">
+        <f t="shared" si="0"/>
+        <v>Done</v>
+      </c>
+      <c r="B5" s="7">
+        <v>44022</v>
+      </c>
+      <c r="C5" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" t="s">
+        <v>89</v>
+      </c>
+      <c r="E5" t="s">
+        <v>100</v>
+      </c>
+      <c r="F5" t="str">
+        <f t="shared" si="1"/>
+        <v>Done</v>
+      </c>
+      <c r="G5" s="7">
+        <v>44022</v>
+      </c>
+      <c r="H5" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="I5" t="s">
+        <v>89</v>
+      </c>
+      <c r="J5" t="s">
+        <v>100</v>
+      </c>
+      <c r="K5" t="str">
+        <f t="shared" si="2"/>
+        <v>Done</v>
+      </c>
+      <c r="L5" s="7">
+        <v>44022</v>
+      </c>
+      <c r="M5" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="N5" t="s">
+        <v>89</v>
+      </c>
+      <c r="O5" t="s">
+        <v>100</v>
+      </c>
+      <c r="P5" t="str">
+        <f t="shared" si="3"/>
+        <v>Done</v>
+      </c>
+      <c r="Q5" s="7">
+        <v>44022</v>
+      </c>
+      <c r="R5" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="S5" t="s">
+        <v>89</v>
+      </c>
+      <c r="T5" t="s">
+        <v>100</v>
+      </c>
+      <c r="U5" t="str">
+        <f t="shared" si="4"/>
+        <v>Done</v>
+      </c>
+      <c r="V5" s="7">
+        <v>44022</v>
+      </c>
+      <c r="W5" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="X5" t="s">
+        <v>89</v>
+      </c>
+      <c r="Y5" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A6" t="str">
+        <f t="shared" si="0"/>
+        <v>Pending</v>
+      </c>
+      <c r="C6" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" t="s">
+        <v>96</v>
+      </c>
+      <c r="E6" t="s">
+        <v>86</v>
+      </c>
+      <c r="F6" t="str">
+        <f t="shared" si="1"/>
+        <v>Pending</v>
+      </c>
+      <c r="H6" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="I6" t="s">
+        <v>96</v>
+      </c>
+      <c r="J6" t="s">
+        <v>86</v>
+      </c>
+      <c r="K6" t="str">
+        <f t="shared" si="2"/>
+        <v>Pending</v>
+      </c>
+      <c r="M6" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="N6" t="s">
+        <v>96</v>
+      </c>
+      <c r="O6" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="P6" t="str">
+        <f t="shared" si="3"/>
+        <v>Pending</v>
+      </c>
+      <c r="R6" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="S6" t="s">
+        <v>96</v>
+      </c>
+      <c r="T6" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="U6" t="str">
+        <f t="shared" si="4"/>
+        <v>Pending</v>
+      </c>
+      <c r="W6" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="X6" t="s">
+        <v>96</v>
+      </c>
+      <c r="Y6" s="1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A7" t="str">
+        <f t="shared" si="0"/>
+        <v>Pending</v>
+      </c>
+      <c r="C7" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D7" t="s">
         <v>76</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="E7" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="F4" s="15" t="s">
+      <c r="F7" t="str">
+        <f t="shared" si="1"/>
+        <v>Pending</v>
+      </c>
+      <c r="H7" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="G4" t="s">
+      <c r="I7" t="s">
         <v>76</v>
       </c>
-      <c r="H4" s="1" t="s">
+      <c r="J7" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="I4" s="15" t="s">
+      <c r="K7" t="str">
+        <f t="shared" si="2"/>
+        <v>Pending</v>
+      </c>
+      <c r="M7" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="J4" t="s">
+      <c r="N7" t="s">
         <v>76</v>
       </c>
-      <c r="K4" s="1" t="s">
+      <c r="O7" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="L4" s="15" t="s">
+      <c r="P7" t="str">
+        <f t="shared" si="3"/>
+        <v>Pending</v>
+      </c>
+      <c r="R7" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="M4" t="s">
+      <c r="S7" t="s">
         <v>76</v>
       </c>
-      <c r="N4" s="1" t="s">
+      <c r="T7" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="O4" s="15" t="s">
+      <c r="U7" t="str">
+        <f t="shared" si="4"/>
+        <v>Pending</v>
+      </c>
+      <c r="W7" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="P4" t="s">
+      <c r="X7" t="s">
         <v>76</v>
       </c>
-      <c r="Q4" s="1" t="s">
+      <c r="Y7" s="1" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>101</v>
-      </c>
-      <c r="C5" s="14" t="s">
+    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A8" t="str">
+        <f t="shared" si="0"/>
+        <v>Pending</v>
+      </c>
+      <c r="C8" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D8" t="s">
         <v>80</v>
       </c>
-      <c r="E5" t="s">
-        <v>87</v>
-      </c>
-      <c r="F5" s="14" t="s">
+      <c r="E8" t="s">
+        <v>86</v>
+      </c>
+      <c r="F8" t="str">
+        <f t="shared" si="1"/>
+        <v>Pending</v>
+      </c>
+      <c r="H8" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="G5" t="s">
+      <c r="I8" t="s">
         <v>80</v>
-      </c>
-      <c r="H5" t="s">
-        <v>87</v>
-      </c>
-      <c r="I5" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="J5" t="s">
-        <v>80</v>
-      </c>
-      <c r="K5" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="L5" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="M5" t="s">
-        <v>80</v>
-      </c>
-      <c r="N5" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="O5" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="P5" t="s">
-        <v>80</v>
-      </c>
-      <c r="Q5" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>101</v>
-      </c>
-      <c r="C6" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="D6" t="s">
-        <v>83</v>
-      </c>
-      <c r="E6" t="s">
-        <v>87</v>
-      </c>
-      <c r="F6" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="G6" t="s">
-        <v>83</v>
-      </c>
-      <c r="H6" t="s">
-        <v>87</v>
-      </c>
-      <c r="I6" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="J6" t="s">
-        <v>83</v>
-      </c>
-      <c r="K6" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="L6" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="M6" t="s">
-        <v>83</v>
-      </c>
-      <c r="N6" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="O6" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="P6" t="s">
-        <v>83</v>
-      </c>
-      <c r="Q6" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>101</v>
-      </c>
-      <c r="C7" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="D7" t="s">
-        <v>13</v>
-      </c>
-      <c r="E7" t="s">
-        <v>85</v>
-      </c>
-      <c r="F7" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="G7" t="s">
-        <v>13</v>
-      </c>
-      <c r="H7" t="s">
-        <v>85</v>
-      </c>
-      <c r="I7" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="J7" t="s">
-        <v>13</v>
-      </c>
-      <c r="K7" t="s">
-        <v>85</v>
-      </c>
-      <c r="L7" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="M7" t="s">
-        <v>13</v>
-      </c>
-      <c r="N7" t="s">
-        <v>85</v>
-      </c>
-      <c r="O7" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="P7" t="s">
-        <v>13</v>
-      </c>
-      <c r="Q7" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>101</v>
-      </c>
-      <c r="C8" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="D8" t="s">
-        <v>86</v>
-      </c>
-      <c r="E8" t="s">
-        <v>87</v>
-      </c>
-      <c r="F8" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="G8" t="s">
-        <v>86</v>
-      </c>
-      <c r="H8" t="s">
-        <v>87</v>
-      </c>
-      <c r="I8" s="14" t="s">
-        <v>9</v>
       </c>
       <c r="J8" t="s">
         <v>86</v>
       </c>
-      <c r="K8" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="L8" s="14" t="s">
+      <c r="K8" t="str">
+        <f t="shared" si="2"/>
+        <v>Pending</v>
+      </c>
+      <c r="M8" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="N8" t="s">
+        <v>80</v>
+      </c>
+      <c r="O8" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="P8" t="str">
+        <f t="shared" si="3"/>
+        <v>Pending</v>
+      </c>
+      <c r="R8" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="S8" t="s">
+        <v>80</v>
+      </c>
+      <c r="T8" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="U8" t="str">
+        <f t="shared" si="4"/>
+        <v>Pending</v>
+      </c>
+      <c r="W8" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="X8" t="s">
+        <v>80</v>
+      </c>
+      <c r="Y8" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A9" t="str">
+        <f t="shared" si="0"/>
+        <v>Pending</v>
+      </c>
+      <c r="C9" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="M8" t="s">
+      <c r="D9" t="s">
+        <v>85</v>
+      </c>
+      <c r="E9" t="s">
         <v>86</v>
       </c>
-      <c r="N8" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="O8" s="14" t="s">
+      <c r="F9" t="str">
+        <f t="shared" si="1"/>
+        <v>Pending</v>
+      </c>
+      <c r="H9" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="P8" t="s">
+      <c r="I9" t="s">
+        <v>85</v>
+      </c>
+      <c r="J9" t="s">
         <v>86</v>
       </c>
-      <c r="Q8" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>101</v>
-      </c>
-      <c r="C9" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="D9" t="s">
-        <v>90</v>
-      </c>
-      <c r="E9" t="s">
-        <v>85</v>
-      </c>
-      <c r="F9" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="G9" t="s">
-        <v>90</v>
-      </c>
-      <c r="H9" t="s">
-        <v>85</v>
-      </c>
-      <c r="I9" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="J9" t="s">
-        <v>90</v>
-      </c>
-      <c r="K9" t="s">
-        <v>85</v>
-      </c>
-      <c r="L9" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="M9" t="s">
-        <v>90</v>
+      <c r="K9" t="str">
+        <f t="shared" si="2"/>
+        <v>Pending</v>
+      </c>
+      <c r="M9" s="14" t="s">
+        <v>9</v>
       </c>
       <c r="N9" t="s">
         <v>85</v>
       </c>
-      <c r="O9" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="P9" t="s">
-        <v>90</v>
-      </c>
-      <c r="Q9" t="s">
+      <c r="O9" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="P9" t="str">
+        <f t="shared" si="3"/>
+        <v>Pending</v>
+      </c>
+      <c r="R9" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="S9" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>101</v>
+      <c r="T9" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="U9" t="str">
+        <f t="shared" si="4"/>
+        <v>Pending</v>
+      </c>
+      <c r="W9" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="X9" t="s">
+        <v>85</v>
+      </c>
+      <c r="Y9" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="10" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A10" t="str">
+        <f t="shared" si="0"/>
+        <v>Pending</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="D10" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="E10" t="s">
-        <v>87</v>
-      </c>
-      <c r="F10" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="G10" t="s">
-        <v>91</v>
-      </c>
-      <c r="H10" t="s">
-        <v>87</v>
-      </c>
-      <c r="I10" s="14" t="s">
-        <v>16</v>
+        <v>86</v>
+      </c>
+      <c r="F10" t="str">
+        <f t="shared" si="1"/>
+        <v>Pending</v>
+      </c>
+      <c r="H10" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="I10" t="s">
+        <v>83</v>
       </c>
       <c r="J10" t="s">
-        <v>91</v>
-      </c>
-      <c r="K10" t="s">
-        <v>87</v>
-      </c>
-      <c r="L10" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="M10" t="s">
-        <v>91</v>
-      </c>
-      <c r="N10" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="K10" t="str">
+        <f t="shared" si="2"/>
+        <v>Pending</v>
+      </c>
+      <c r="M10" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="N10" t="s">
+        <v>83</v>
+      </c>
+      <c r="O10" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="P10" t="str">
+        <f t="shared" si="3"/>
+        <v>Pending</v>
+      </c>
+      <c r="R10" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="S10" t="s">
+        <v>83</v>
+      </c>
+      <c r="T10" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="U10" t="str">
+        <f t="shared" si="4"/>
+        <v>Pending</v>
+      </c>
+      <c r="W10" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="X10" t="s">
+        <v>83</v>
+      </c>
+      <c r="Y10" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="11" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A11" t="str">
+        <f t="shared" si="0"/>
+        <v>Pending</v>
+      </c>
+      <c r="C11" s="14" t="s">
         <v>92</v>
       </c>
-      <c r="O10" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="P10" t="s">
-        <v>91</v>
-      </c>
-      <c r="Q10" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>101</v>
-      </c>
-      <c r="C11" s="14" t="s">
+      <c r="D11" t="s">
         <v>93</v>
       </c>
-      <c r="D11" t="s">
+      <c r="E11" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="E11" s="1" t="s">
+      <c r="F11" t="str">
+        <f t="shared" si="1"/>
+        <v>Pending</v>
+      </c>
+      <c r="H11" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="I11" t="s">
+        <v>93</v>
+      </c>
+      <c r="J11" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="K11" t="str">
+        <f t="shared" si="2"/>
+        <v>Pending</v>
+      </c>
+      <c r="M11" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="N11" t="s">
+        <v>93</v>
+      </c>
+      <c r="O11" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="F11" s="14" t="s">
+      <c r="P11" t="str">
+        <f t="shared" si="3"/>
+        <v>Pending</v>
+      </c>
+      <c r="R11" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="S11" t="s">
         <v>93</v>
       </c>
-      <c r="G11" t="s">
-        <v>94</v>
-      </c>
-      <c r="H11" s="1" t="s">
+      <c r="T11" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="I11" s="14" t="s">
+      <c r="U11" t="str">
+        <f t="shared" si="4"/>
+        <v>Pending</v>
+      </c>
+      <c r="W11" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="X11" t="s">
         <v>93</v>
       </c>
-      <c r="J11" t="s">
-        <v>94</v>
-      </c>
-      <c r="K11" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="L11" s="14" t="s">
-        <v>93</v>
-      </c>
-      <c r="M11" t="s">
-        <v>94</v>
-      </c>
-      <c r="N11" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="O11" s="14" t="s">
-        <v>93</v>
-      </c>
-      <c r="P11" t="s">
-        <v>94</v>
-      </c>
-      <c r="Q11" s="1" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>101</v>
+      <c r="Y11" s="1" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="12" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A12" t="str">
+        <f>IF(ISBLANK(B12),"Pending","Done")</f>
+        <v>Done</v>
+      </c>
+      <c r="B12" s="7">
+        <v>44022</v>
       </c>
       <c r="C12" s="14" t="s">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="D12" t="s">
-        <v>97</v>
+        <v>30</v>
       </c>
       <c r="E12" t="s">
-        <v>87</v>
-      </c>
-      <c r="F12" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="G12" t="s">
-        <v>97</v>
-      </c>
-      <c r="H12" t="s">
-        <v>87</v>
-      </c>
-      <c r="I12" s="14" t="s">
-        <v>15</v>
+        <v>86</v>
+      </c>
+      <c r="F12" t="str">
+        <f>IF(ISBLANK(G12),"Pending","Done")</f>
+        <v>Done</v>
+      </c>
+      <c r="G12" s="7">
+        <v>44022</v>
+      </c>
+      <c r="H12" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="I12" t="s">
+        <v>30</v>
       </c>
       <c r="J12" t="s">
-        <v>97</v>
-      </c>
-      <c r="K12" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="L12" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="M12" t="s">
-        <v>97</v>
-      </c>
-      <c r="N12" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="O12" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="P12" t="s">
-        <v>97</v>
-      </c>
-      <c r="Q12" s="1" t="s">
-        <v>98</v>
+        <v>86</v>
+      </c>
+      <c r="K12" t="str">
+        <f>IF(ISBLANK(L12),"Pending","Done")</f>
+        <v>Done</v>
+      </c>
+      <c r="L12" s="7">
+        <v>44022</v>
+      </c>
+      <c r="M12" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="N12" t="s">
+        <v>30</v>
+      </c>
+      <c r="O12" t="s">
+        <v>86</v>
+      </c>
+      <c r="P12" t="str">
+        <f>IF(ISBLANK(Q12),"Pending","Done")</f>
+        <v>Done</v>
+      </c>
+      <c r="Q12" s="7">
+        <v>44022</v>
+      </c>
+      <c r="R12" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="S12" t="s">
+        <v>30</v>
+      </c>
+      <c r="T12" t="s">
+        <v>86</v>
+      </c>
+      <c r="U12" t="str">
+        <f>IF(ISBLANK(V12),"Pending","Done")</f>
+        <v>Done</v>
+      </c>
+      <c r="V12" s="7">
+        <v>44022</v>
+      </c>
+      <c r="W12" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="X12" t="s">
+        <v>30</v>
+      </c>
+      <c r="Y12" t="s">
+        <v>86</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2:B12">
+    <cfRule type="cellIs" dxfId="9" priority="9" operator="equal">
+      <formula>"Pending"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="8" priority="10" operator="equal">
+      <formula>"Done"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F2:G12">
+    <cfRule type="cellIs" dxfId="7" priority="7" operator="equal">
+      <formula>"Pending"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="6" priority="8" operator="equal">
+      <formula>"Done"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K2:L12">
+    <cfRule type="cellIs" dxfId="5" priority="5" operator="equal">
+      <formula>"Pending"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="4" priority="6" operator="equal">
+      <formula>"Done"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="P2:Q12">
+    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
+      <formula>"Pending"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="4" operator="equal">
+      <formula>"Done"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="U2:V12">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>

</xml_diff>

<commit_message>
portal inmobiliario transform done
</commit_message>
<xml_diff>
--- a/data/T/byHand/housesSmart.xlsx
+++ b/data/T/byHand/housesSmart.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Reference\housemodel\data\T\byHand\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08B3821A-7A6C-45B9-BAC3-71BB396129D8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{774EFE18-F61B-4CBD-8250-7B349CA453B5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7200" yWindow="0" windowWidth="21600" windowHeight="15600" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Columns" sheetId="1" r:id="rId1"/>
@@ -737,77 +737,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="124">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="114">
     <dxf>
       <fill>
         <patternFill>
@@ -2576,7 +2506,7 @@
   <dimension ref="A1:Y66"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="V20" sqref="V20"/>
+      <selection activeCell="B21" sqref="B21:B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3945,7 +3875,10 @@
     <row r="21" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A21" t="str">
         <f t="shared" si="5"/>
-        <v>Pending</v>
+        <v>Done</v>
+      </c>
+      <c r="B21" s="7">
+        <v>44025</v>
       </c>
       <c r="C21" s="27" t="s">
         <v>15</v>
@@ -3997,7 +3930,10 @@
     <row r="22" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A22" t="str">
         <f t="shared" si="5"/>
-        <v>Pending</v>
+        <v>Done</v>
+      </c>
+      <c r="B22" s="7">
+        <v>44025</v>
       </c>
       <c r="C22" s="27" t="s">
         <v>6</v>
@@ -4049,7 +3985,10 @@
     <row r="23" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A23" t="str">
         <f t="shared" si="5"/>
-        <v>Pending</v>
+        <v>Done</v>
+      </c>
+      <c r="B23" s="7">
+        <v>44025</v>
       </c>
       <c r="C23" s="27" t="s">
         <v>8</v>
@@ -4101,7 +4040,10 @@
     <row r="24" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A24" t="str">
         <f t="shared" si="5"/>
-        <v>Pending</v>
+        <v>Done</v>
+      </c>
+      <c r="B24" s="7">
+        <v>44025</v>
       </c>
       <c r="C24" s="27" t="s">
         <v>9</v>
@@ -4153,7 +4095,10 @@
     <row r="25" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A25" t="str">
         <f t="shared" si="5"/>
-        <v>Pending</v>
+        <v>Done</v>
+      </c>
+      <c r="B25" s="7">
+        <v>44025</v>
       </c>
       <c r="C25" s="27" t="s">
         <v>10</v>
@@ -4205,9 +4150,11 @@
     <row r="26" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A26" t="str">
         <f>IF(ISBLANK(B26),"Pending","Done")</f>
-        <v>Pending</v>
-      </c>
-      <c r="B26" s="7"/>
+        <v>Done</v>
+      </c>
+      <c r="B26" s="7">
+        <v>44025</v>
+      </c>
       <c r="C26" s="27" t="s">
         <v>92</v>
       </c>
@@ -6785,362 +6732,362 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A3:B13">
-    <cfRule type="cellIs" dxfId="123" priority="123" operator="equal">
+    <cfRule type="cellIs" dxfId="113" priority="123" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="122" priority="124" operator="equal">
+    <cfRule type="cellIs" dxfId="112" priority="124" operator="equal">
       <formula>"Done"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F3:G4 F6:G6 F5 F13:G13 F7:F12">
-    <cfRule type="cellIs" dxfId="121" priority="121" operator="equal">
+    <cfRule type="cellIs" dxfId="111" priority="121" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="120" priority="122" operator="equal">
+    <cfRule type="cellIs" dxfId="110" priority="122" operator="equal">
       <formula>"Done"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K3:L4 K6:L6 K5 K13:L13 K7:K12">
-    <cfRule type="cellIs" dxfId="119" priority="119" operator="equal">
+    <cfRule type="cellIs" dxfId="109" priority="119" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="118" priority="120" operator="equal">
+    <cfRule type="cellIs" dxfId="108" priority="120" operator="equal">
       <formula>"Done"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P3:Q4 P6:Q6 P5 P13:Q13 P7:P12">
-    <cfRule type="cellIs" dxfId="117" priority="117" operator="equal">
+    <cfRule type="cellIs" dxfId="107" priority="117" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="116" priority="118" operator="equal">
+    <cfRule type="cellIs" dxfId="106" priority="118" operator="equal">
       <formula>"Done"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U3:V4 U6:V6 U5 U13:V13 U7:U12">
-    <cfRule type="cellIs" dxfId="115" priority="115" operator="equal">
+    <cfRule type="cellIs" dxfId="105" priority="115" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="114" priority="116" operator="equal">
+    <cfRule type="cellIs" dxfId="104" priority="116" operator="equal">
       <formula>"Done"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A16:B27">
-    <cfRule type="cellIs" dxfId="113" priority="113" operator="equal">
+    <cfRule type="cellIs" dxfId="103" priority="113" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="112" priority="114" operator="equal">
+    <cfRule type="cellIs" dxfId="102" priority="114" operator="equal">
       <formula>"Done"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F16:F26">
-    <cfRule type="cellIs" dxfId="111" priority="111" operator="equal">
+    <cfRule type="cellIs" dxfId="101" priority="111" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="110" priority="112" operator="equal">
+    <cfRule type="cellIs" dxfId="100" priority="112" operator="equal">
       <formula>"Done"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K16:K26">
-    <cfRule type="cellIs" dxfId="109" priority="109" operator="equal">
+    <cfRule type="cellIs" dxfId="99" priority="109" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="108" priority="110" operator="equal">
+    <cfRule type="cellIs" dxfId="98" priority="110" operator="equal">
       <formula>"Done"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P16:P26">
-    <cfRule type="cellIs" dxfId="107" priority="107" operator="equal">
+    <cfRule type="cellIs" dxfId="97" priority="107" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="106" priority="108" operator="equal">
+    <cfRule type="cellIs" dxfId="96" priority="108" operator="equal">
       <formula>"Done"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U16:U26">
-    <cfRule type="cellIs" dxfId="105" priority="105" operator="equal">
+    <cfRule type="cellIs" dxfId="95" priority="105" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="104" priority="106" operator="equal">
+    <cfRule type="cellIs" dxfId="94" priority="106" operator="equal">
       <formula>"Done"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G5">
-    <cfRule type="cellIs" dxfId="95" priority="93" operator="equal">
+    <cfRule type="cellIs" dxfId="93" priority="93" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="94" priority="94" operator="equal">
+    <cfRule type="cellIs" dxfId="92" priority="94" operator="equal">
       <formula>"Done"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G7:G12">
-    <cfRule type="cellIs" dxfId="93" priority="91" operator="equal">
+    <cfRule type="cellIs" dxfId="91" priority="91" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="92" priority="92" operator="equal">
+    <cfRule type="cellIs" dxfId="90" priority="92" operator="equal">
       <formula>"Done"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L5">
-    <cfRule type="cellIs" dxfId="91" priority="89" operator="equal">
+    <cfRule type="cellIs" dxfId="89" priority="89" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="90" priority="90" operator="equal">
+    <cfRule type="cellIs" dxfId="88" priority="90" operator="equal">
       <formula>"Done"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L7:L12">
-    <cfRule type="cellIs" dxfId="89" priority="87" operator="equal">
+    <cfRule type="cellIs" dxfId="87" priority="87" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="88" priority="88" operator="equal">
+    <cfRule type="cellIs" dxfId="86" priority="88" operator="equal">
       <formula>"Done"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q5">
-    <cfRule type="cellIs" dxfId="87" priority="85" operator="equal">
+    <cfRule type="cellIs" dxfId="85" priority="85" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="86" priority="86" operator="equal">
+    <cfRule type="cellIs" dxfId="84" priority="86" operator="equal">
       <formula>"Done"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q7:Q12">
-    <cfRule type="cellIs" dxfId="85" priority="83" operator="equal">
+    <cfRule type="cellIs" dxfId="83" priority="83" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="84" priority="84" operator="equal">
+    <cfRule type="cellIs" dxfId="82" priority="84" operator="equal">
       <formula>"Done"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V5">
-    <cfRule type="cellIs" dxfId="83" priority="81" operator="equal">
+    <cfRule type="cellIs" dxfId="81" priority="81" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="82" priority="82" operator="equal">
+    <cfRule type="cellIs" dxfId="80" priority="82" operator="equal">
       <formula>"Done"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V7:V12">
-    <cfRule type="cellIs" dxfId="81" priority="79" operator="equal">
+    <cfRule type="cellIs" dxfId="79" priority="79" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="80" priority="80" operator="equal">
+    <cfRule type="cellIs" dxfId="78" priority="80" operator="equal">
       <formula>"Done"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A30:B40">
-    <cfRule type="cellIs" dxfId="79" priority="77" operator="equal">
+    <cfRule type="cellIs" dxfId="77" priority="77" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="78" priority="78" operator="equal">
+    <cfRule type="cellIs" dxfId="76" priority="78" operator="equal">
       <formula>"Done"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F30:F40">
-    <cfRule type="cellIs" dxfId="77" priority="75" operator="equal">
+    <cfRule type="cellIs" dxfId="75" priority="75" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="76" priority="76" operator="equal">
+    <cfRule type="cellIs" dxfId="74" priority="76" operator="equal">
       <formula>"Done"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K30:K40">
-    <cfRule type="cellIs" dxfId="75" priority="73" operator="equal">
+    <cfRule type="cellIs" dxfId="73" priority="73" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="74" priority="74" operator="equal">
+    <cfRule type="cellIs" dxfId="72" priority="74" operator="equal">
       <formula>"Done"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P30:P40">
-    <cfRule type="cellIs" dxfId="73" priority="71" operator="equal">
+    <cfRule type="cellIs" dxfId="71" priority="71" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="72" priority="72" operator="equal">
+    <cfRule type="cellIs" dxfId="70" priority="72" operator="equal">
       <formula>"Done"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U30:U40">
-    <cfRule type="cellIs" dxfId="71" priority="69" operator="equal">
+    <cfRule type="cellIs" dxfId="69" priority="69" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="70" priority="70" operator="equal">
+    <cfRule type="cellIs" dxfId="68" priority="70" operator="equal">
       <formula>"Done"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G30:G40">
-    <cfRule type="cellIs" dxfId="69" priority="67" operator="equal">
+    <cfRule type="cellIs" dxfId="67" priority="67" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="68" priority="68" operator="equal">
+    <cfRule type="cellIs" dxfId="66" priority="68" operator="equal">
       <formula>"Done"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L30:L40">
-    <cfRule type="cellIs" dxfId="67" priority="65" operator="equal">
+    <cfRule type="cellIs" dxfId="65" priority="65" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="66" priority="66" operator="equal">
+    <cfRule type="cellIs" dxfId="64" priority="66" operator="equal">
       <formula>"Done"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q30:Q40">
-    <cfRule type="cellIs" dxfId="65" priority="63" operator="equal">
+    <cfRule type="cellIs" dxfId="63" priority="63" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="64" priority="64" operator="equal">
+    <cfRule type="cellIs" dxfId="62" priority="64" operator="equal">
       <formula>"Done"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V30:V40">
-    <cfRule type="cellIs" dxfId="63" priority="61" operator="equal">
+    <cfRule type="cellIs" dxfId="61" priority="61" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="62" priority="62" operator="equal">
+    <cfRule type="cellIs" dxfId="60" priority="62" operator="equal">
       <formula>"Done"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A43:B53">
-    <cfRule type="cellIs" dxfId="61" priority="59" operator="equal">
+    <cfRule type="cellIs" dxfId="59" priority="59" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="60" priority="60" operator="equal">
+    <cfRule type="cellIs" dxfId="58" priority="60" operator="equal">
       <formula>"Done"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F43:F53">
-    <cfRule type="cellIs" dxfId="59" priority="57" operator="equal">
+    <cfRule type="cellIs" dxfId="57" priority="57" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="58" priority="58" operator="equal">
+    <cfRule type="cellIs" dxfId="56" priority="58" operator="equal">
       <formula>"Done"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K43:K53">
-    <cfRule type="cellIs" dxfId="57" priority="55" operator="equal">
+    <cfRule type="cellIs" dxfId="55" priority="55" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="56" priority="56" operator="equal">
+    <cfRule type="cellIs" dxfId="54" priority="56" operator="equal">
       <formula>"Done"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P43:P53">
-    <cfRule type="cellIs" dxfId="55" priority="53" operator="equal">
+    <cfRule type="cellIs" dxfId="53" priority="53" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="54" priority="54" operator="equal">
+    <cfRule type="cellIs" dxfId="52" priority="54" operator="equal">
       <formula>"Done"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U43:U53">
-    <cfRule type="cellIs" dxfId="53" priority="51" operator="equal">
+    <cfRule type="cellIs" dxfId="51" priority="51" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="52" priority="52" operator="equal">
+    <cfRule type="cellIs" dxfId="50" priority="52" operator="equal">
       <formula>"Done"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G43:G53">
-    <cfRule type="cellIs" dxfId="51" priority="49" operator="equal">
+    <cfRule type="cellIs" dxfId="49" priority="49" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="50" priority="50" operator="equal">
+    <cfRule type="cellIs" dxfId="48" priority="50" operator="equal">
       <formula>"Done"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L43:L53">
-    <cfRule type="cellIs" dxfId="49" priority="47" operator="equal">
+    <cfRule type="cellIs" dxfId="47" priority="47" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="48" priority="48" operator="equal">
+    <cfRule type="cellIs" dxfId="46" priority="48" operator="equal">
       <formula>"Done"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q43:Q53">
-    <cfRule type="cellIs" dxfId="47" priority="45" operator="equal">
+    <cfRule type="cellIs" dxfId="45" priority="45" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="46" priority="46" operator="equal">
+    <cfRule type="cellIs" dxfId="44" priority="46" operator="equal">
       <formula>"Done"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V43:V53">
-    <cfRule type="cellIs" dxfId="45" priority="43" operator="equal">
+    <cfRule type="cellIs" dxfId="43" priority="43" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="44" priority="44" operator="equal">
+    <cfRule type="cellIs" dxfId="42" priority="44" operator="equal">
       <formula>"Done"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A56:B66">
-    <cfRule type="cellIs" dxfId="43" priority="41" operator="equal">
+    <cfRule type="cellIs" dxfId="41" priority="41" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="42" priority="42" operator="equal">
+    <cfRule type="cellIs" dxfId="40" priority="42" operator="equal">
       <formula>"Done"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F56:F66">
-    <cfRule type="cellIs" dxfId="41" priority="39" operator="equal">
+    <cfRule type="cellIs" dxfId="39" priority="39" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="40" priority="40" operator="equal">
+    <cfRule type="cellIs" dxfId="38" priority="40" operator="equal">
       <formula>"Done"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K56:K66">
-    <cfRule type="cellIs" dxfId="39" priority="37" operator="equal">
+    <cfRule type="cellIs" dxfId="37" priority="37" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="38" priority="38" operator="equal">
+    <cfRule type="cellIs" dxfId="36" priority="38" operator="equal">
       <formula>"Done"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P56:P66">
-    <cfRule type="cellIs" dxfId="37" priority="35" operator="equal">
+    <cfRule type="cellIs" dxfId="35" priority="35" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="36" priority="36" operator="equal">
+    <cfRule type="cellIs" dxfId="34" priority="36" operator="equal">
       <formula>"Done"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U56:U66">
-    <cfRule type="cellIs" dxfId="35" priority="33" operator="equal">
+    <cfRule type="cellIs" dxfId="33" priority="33" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="34" priority="34" operator="equal">
+    <cfRule type="cellIs" dxfId="32" priority="34" operator="equal">
       <formula>"Done"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G56:G66">
-    <cfRule type="cellIs" dxfId="33" priority="31" operator="equal">
+    <cfRule type="cellIs" dxfId="31" priority="31" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="32" priority="32" operator="equal">
+    <cfRule type="cellIs" dxfId="30" priority="32" operator="equal">
       <formula>"Done"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L56:L66">
-    <cfRule type="cellIs" dxfId="31" priority="29" operator="equal">
+    <cfRule type="cellIs" dxfId="29" priority="29" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="30" priority="30" operator="equal">
+    <cfRule type="cellIs" dxfId="28" priority="30" operator="equal">
       <formula>"Done"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q56:Q66">
-    <cfRule type="cellIs" dxfId="29" priority="27" operator="equal">
+    <cfRule type="cellIs" dxfId="27" priority="27" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="28" priority="28" operator="equal">
+    <cfRule type="cellIs" dxfId="26" priority="28" operator="equal">
       <formula>"Done"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V56:V66">
-    <cfRule type="cellIs" dxfId="27" priority="25" operator="equal">
+    <cfRule type="cellIs" dxfId="25" priority="25" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="26" priority="26" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="26" operator="equal">
       <formula>"Done"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
format for toctoc done
</commit_message>
<xml_diff>
--- a/data/T/byHand/housesSmart.xlsx
+++ b/data/T/byHand/housesSmart.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Reference\housemodel\data\T\byHand\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{774EFE18-F61B-4CBD-8250-7B349CA453B5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6ECDBD20-979C-4444-9C91-6E0B23E577B4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="7200" yWindow="0" windowWidth="21600" windowHeight="15600" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -737,7 +737,21 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="114">
+  <dxfs count="116">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -2506,7 +2520,7 @@
   <dimension ref="A1:Y66"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21:B26"/>
+      <selection activeCell="G19" sqref="G19:G26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3762,9 +3776,11 @@
       </c>
       <c r="F19" t="str">
         <f t="shared" si="6"/>
-        <v>Pending</v>
-      </c>
-      <c r="G19" s="7"/>
+        <v>Done</v>
+      </c>
+      <c r="G19" s="7">
+        <v>44025</v>
+      </c>
       <c r="H19" s="27" t="s">
         <v>16</v>
       </c>
@@ -3888,7 +3904,10 @@
       </c>
       <c r="F21" t="str">
         <f t="shared" si="6"/>
-        <v>Pending</v>
+        <v>Done</v>
+      </c>
+      <c r="G21" s="7">
+        <v>44025</v>
       </c>
       <c r="H21" s="27" t="s">
         <v>15</v>
@@ -3943,7 +3962,10 @@
       </c>
       <c r="F22" t="str">
         <f t="shared" si="6"/>
-        <v>Pending</v>
+        <v>Done</v>
+      </c>
+      <c r="G22" s="7">
+        <v>44025</v>
       </c>
       <c r="H22" s="27" t="s">
         <v>6</v>
@@ -3998,7 +4020,10 @@
       </c>
       <c r="F23" t="str">
         <f t="shared" si="6"/>
-        <v>Pending</v>
+        <v>Done</v>
+      </c>
+      <c r="G23" s="7">
+        <v>44025</v>
       </c>
       <c r="H23" s="27" t="s">
         <v>8</v>
@@ -4053,7 +4078,10 @@
       </c>
       <c r="F24" t="str">
         <f t="shared" si="6"/>
-        <v>Pending</v>
+        <v>Done</v>
+      </c>
+      <c r="G24" s="7">
+        <v>44025</v>
       </c>
       <c r="H24" s="27" t="s">
         <v>9</v>
@@ -4108,7 +4136,10 @@
       </c>
       <c r="F25" t="str">
         <f t="shared" si="6"/>
-        <v>Pending</v>
+        <v>Done</v>
+      </c>
+      <c r="G25" s="7">
+        <v>44025</v>
       </c>
       <c r="H25" s="27" t="s">
         <v>10</v>
@@ -4163,9 +4194,11 @@
       </c>
       <c r="F26" t="str">
         <f>IF(ISBLANK(G26),"Pending","Done")</f>
-        <v>Pending</v>
-      </c>
-      <c r="G26" s="7"/>
+        <v>Done</v>
+      </c>
+      <c r="G26" s="7">
+        <v>44025</v>
+      </c>
       <c r="H26" s="27" t="s">
         <v>92</v>
       </c>
@@ -6732,6 +6765,14 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A3:B13">
+    <cfRule type="cellIs" dxfId="115" priority="125" operator="equal">
+      <formula>"Pending"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="114" priority="126" operator="equal">
+      <formula>"Done"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F3:G4 F6:G6 F5 F13:G13 F7:F12">
     <cfRule type="cellIs" dxfId="113" priority="123" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
@@ -6739,7 +6780,7 @@
       <formula>"Done"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F3:G4 F6:G6 F5 F13:G13 F7:F12">
+  <conditionalFormatting sqref="K3:L4 K6:L6 K5 K13:L13 K7:K12">
     <cfRule type="cellIs" dxfId="111" priority="121" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
@@ -6747,7 +6788,7 @@
       <formula>"Done"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K3:L4 K6:L6 K5 K13:L13 K7:K12">
+  <conditionalFormatting sqref="P3:Q4 P6:Q6 P5 P13:Q13 P7:P12">
     <cfRule type="cellIs" dxfId="109" priority="119" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
@@ -6755,7 +6796,7 @@
       <formula>"Done"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="P3:Q4 P6:Q6 P5 P13:Q13 P7:P12">
+  <conditionalFormatting sqref="U3:V4 U6:V6 U5 U13:V13 U7:U12">
     <cfRule type="cellIs" dxfId="107" priority="117" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
@@ -6763,7 +6804,7 @@
       <formula>"Done"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="U3:V4 U6:V6 U5 U13:V13 U7:U12">
+  <conditionalFormatting sqref="A16:B27">
     <cfRule type="cellIs" dxfId="105" priority="115" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
@@ -6771,7 +6812,7 @@
       <formula>"Done"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A16:B27">
+  <conditionalFormatting sqref="F16:F26">
     <cfRule type="cellIs" dxfId="103" priority="113" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
@@ -6779,7 +6820,7 @@
       <formula>"Done"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F16:F26">
+  <conditionalFormatting sqref="K16:K26">
     <cfRule type="cellIs" dxfId="101" priority="111" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
@@ -6787,7 +6828,7 @@
       <formula>"Done"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K16:K26">
+  <conditionalFormatting sqref="P16:P26">
     <cfRule type="cellIs" dxfId="99" priority="109" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
@@ -6795,7 +6836,7 @@
       <formula>"Done"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="P16:P26">
+  <conditionalFormatting sqref="U16:U26">
     <cfRule type="cellIs" dxfId="97" priority="107" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
@@ -6803,15 +6844,15 @@
       <formula>"Done"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="U16:U26">
-    <cfRule type="cellIs" dxfId="95" priority="105" operator="equal">
+  <conditionalFormatting sqref="G5">
+    <cfRule type="cellIs" dxfId="95" priority="95" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="94" priority="106" operator="equal">
+    <cfRule type="cellIs" dxfId="94" priority="96" operator="equal">
       <formula>"Done"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G5">
+  <conditionalFormatting sqref="G7:G12">
     <cfRule type="cellIs" dxfId="93" priority="93" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
@@ -6819,7 +6860,7 @@
       <formula>"Done"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G7:G12">
+  <conditionalFormatting sqref="L5">
     <cfRule type="cellIs" dxfId="91" priority="91" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
@@ -6827,7 +6868,7 @@
       <formula>"Done"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L5">
+  <conditionalFormatting sqref="L7:L12">
     <cfRule type="cellIs" dxfId="89" priority="89" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
@@ -6835,7 +6876,7 @@
       <formula>"Done"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L7:L12">
+  <conditionalFormatting sqref="Q5">
     <cfRule type="cellIs" dxfId="87" priority="87" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
@@ -6843,7 +6884,7 @@
       <formula>"Done"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Q5">
+  <conditionalFormatting sqref="Q7:Q12">
     <cfRule type="cellIs" dxfId="85" priority="85" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
@@ -6851,7 +6892,7 @@
       <formula>"Done"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Q7:Q12">
+  <conditionalFormatting sqref="V5">
     <cfRule type="cellIs" dxfId="83" priority="83" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
@@ -6859,7 +6900,7 @@
       <formula>"Done"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="V5">
+  <conditionalFormatting sqref="V7:V12">
     <cfRule type="cellIs" dxfId="81" priority="81" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
@@ -6867,7 +6908,7 @@
       <formula>"Done"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="V7:V12">
+  <conditionalFormatting sqref="A30:B40">
     <cfRule type="cellIs" dxfId="79" priority="79" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
@@ -6875,7 +6916,7 @@
       <formula>"Done"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A30:B40">
+  <conditionalFormatting sqref="F30:F40">
     <cfRule type="cellIs" dxfId="77" priority="77" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
@@ -6883,7 +6924,7 @@
       <formula>"Done"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F30:F40">
+  <conditionalFormatting sqref="K30:K40">
     <cfRule type="cellIs" dxfId="75" priority="75" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
@@ -6891,7 +6932,7 @@
       <formula>"Done"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K30:K40">
+  <conditionalFormatting sqref="P30:P40">
     <cfRule type="cellIs" dxfId="73" priority="73" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
@@ -6899,7 +6940,7 @@
       <formula>"Done"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="P30:P40">
+  <conditionalFormatting sqref="U30:U40">
     <cfRule type="cellIs" dxfId="71" priority="71" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
@@ -6907,7 +6948,7 @@
       <formula>"Done"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="U30:U40">
+  <conditionalFormatting sqref="G30:G40">
     <cfRule type="cellIs" dxfId="69" priority="69" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
@@ -6915,7 +6956,7 @@
       <formula>"Done"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G30:G40">
+  <conditionalFormatting sqref="L30:L40">
     <cfRule type="cellIs" dxfId="67" priority="67" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
@@ -6923,7 +6964,7 @@
       <formula>"Done"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L30:L40">
+  <conditionalFormatting sqref="Q30:Q40">
     <cfRule type="cellIs" dxfId="65" priority="65" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
@@ -6931,7 +6972,7 @@
       <formula>"Done"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Q30:Q40">
+  <conditionalFormatting sqref="V30:V40">
     <cfRule type="cellIs" dxfId="63" priority="63" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
@@ -6939,7 +6980,7 @@
       <formula>"Done"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="V30:V40">
+  <conditionalFormatting sqref="A43:B53">
     <cfRule type="cellIs" dxfId="61" priority="61" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
@@ -6947,7 +6988,7 @@
       <formula>"Done"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A43:B53">
+  <conditionalFormatting sqref="F43:F53">
     <cfRule type="cellIs" dxfId="59" priority="59" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
@@ -6955,7 +6996,7 @@
       <formula>"Done"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F43:F53">
+  <conditionalFormatting sqref="K43:K53">
     <cfRule type="cellIs" dxfId="57" priority="57" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
@@ -6963,7 +7004,7 @@
       <formula>"Done"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K43:K53">
+  <conditionalFormatting sqref="P43:P53">
     <cfRule type="cellIs" dxfId="55" priority="55" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
@@ -6971,7 +7012,7 @@
       <formula>"Done"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="P43:P53">
+  <conditionalFormatting sqref="U43:U53">
     <cfRule type="cellIs" dxfId="53" priority="53" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
@@ -6979,7 +7020,7 @@
       <formula>"Done"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="U43:U53">
+  <conditionalFormatting sqref="G43:G53">
     <cfRule type="cellIs" dxfId="51" priority="51" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
@@ -6987,7 +7028,7 @@
       <formula>"Done"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G43:G53">
+  <conditionalFormatting sqref="L43:L53">
     <cfRule type="cellIs" dxfId="49" priority="49" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
@@ -6995,7 +7036,7 @@
       <formula>"Done"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L43:L53">
+  <conditionalFormatting sqref="Q43:Q53">
     <cfRule type="cellIs" dxfId="47" priority="47" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
@@ -7003,7 +7044,7 @@
       <formula>"Done"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Q43:Q53">
+  <conditionalFormatting sqref="V43:V53">
     <cfRule type="cellIs" dxfId="45" priority="45" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
@@ -7011,7 +7052,7 @@
       <formula>"Done"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="V43:V53">
+  <conditionalFormatting sqref="A56:B66">
     <cfRule type="cellIs" dxfId="43" priority="43" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
@@ -7019,7 +7060,7 @@
       <formula>"Done"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A56:B66">
+  <conditionalFormatting sqref="F56:F66">
     <cfRule type="cellIs" dxfId="41" priority="41" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
@@ -7027,7 +7068,7 @@
       <formula>"Done"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F56:F66">
+  <conditionalFormatting sqref="K56:K66">
     <cfRule type="cellIs" dxfId="39" priority="39" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
@@ -7035,7 +7076,7 @@
       <formula>"Done"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K56:K66">
+  <conditionalFormatting sqref="P56:P66">
     <cfRule type="cellIs" dxfId="37" priority="37" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
@@ -7043,7 +7084,7 @@
       <formula>"Done"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="P56:P66">
+  <conditionalFormatting sqref="U56:U66">
     <cfRule type="cellIs" dxfId="35" priority="35" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
@@ -7051,7 +7092,7 @@
       <formula>"Done"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="U56:U66">
+  <conditionalFormatting sqref="G56:G66">
     <cfRule type="cellIs" dxfId="33" priority="33" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
@@ -7059,7 +7100,7 @@
       <formula>"Done"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G56:G66">
+  <conditionalFormatting sqref="L56:L66">
     <cfRule type="cellIs" dxfId="31" priority="31" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
@@ -7067,7 +7108,7 @@
       <formula>"Done"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L56:L66">
+  <conditionalFormatting sqref="Q56:Q66">
     <cfRule type="cellIs" dxfId="29" priority="29" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
@@ -7075,7 +7116,7 @@
       <formula>"Done"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Q56:Q66">
+  <conditionalFormatting sqref="V56:V66">
     <cfRule type="cellIs" dxfId="27" priority="27" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
@@ -7083,7 +7124,7 @@
       <formula>"Done"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="V56:V66">
+  <conditionalFormatting sqref="F27">
     <cfRule type="cellIs" dxfId="25" priority="25" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
@@ -7091,7 +7132,7 @@
       <formula>"Done"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F27">
+  <conditionalFormatting sqref="K27">
     <cfRule type="cellIs" dxfId="23" priority="23" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
@@ -7099,7 +7140,7 @@
       <formula>"Done"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K27">
+  <conditionalFormatting sqref="P27">
     <cfRule type="cellIs" dxfId="21" priority="21" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
@@ -7107,7 +7148,7 @@
       <formula>"Done"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="P27">
+  <conditionalFormatting sqref="U27">
     <cfRule type="cellIs" dxfId="19" priority="19" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
@@ -7115,7 +7156,7 @@
       <formula>"Done"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="U27">
+  <conditionalFormatting sqref="G16:G18 G27">
     <cfRule type="cellIs" dxfId="17" priority="17" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
@@ -7123,7 +7164,7 @@
       <formula>"Done"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G16:G19 G21:G27">
+  <conditionalFormatting sqref="L16:L19 L21:L27">
     <cfRule type="cellIs" dxfId="15" priority="15" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
@@ -7131,7 +7172,7 @@
       <formula>"Done"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L16:L19 L21:L27">
+  <conditionalFormatting sqref="Q16:Q19 Q21:Q27">
     <cfRule type="cellIs" dxfId="13" priority="13" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
@@ -7139,7 +7180,7 @@
       <formula>"Done"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Q16:Q19 Q21:Q27">
+  <conditionalFormatting sqref="V16:V19 V21:V27">
     <cfRule type="cellIs" dxfId="11" priority="11" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
@@ -7147,15 +7188,7 @@
       <formula>"Done"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="V16:V19 V21:V27">
-    <cfRule type="cellIs" dxfId="9" priority="9" operator="equal">
-      <formula>"Pending"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="10" operator="equal">
-      <formula>"Done"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G20">
+  <conditionalFormatting sqref="L20">
     <cfRule type="cellIs" dxfId="7" priority="7" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
@@ -7163,7 +7196,7 @@
       <formula>"Done"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L20">
+  <conditionalFormatting sqref="Q20">
     <cfRule type="cellIs" dxfId="5" priority="5" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
@@ -7171,7 +7204,7 @@
       <formula>"Done"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Q20">
+  <conditionalFormatting sqref="V20">
     <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
@@ -7179,7 +7212,7 @@
       <formula>"Done"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="V20">
+  <conditionalFormatting sqref="G19:G26">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>

</xml_diff>

<commit_message>
like the loly chile propiedades... working on format
</commit_message>
<xml_diff>
--- a/data/T/byHand/housesSmart.xlsx
+++ b/data/T/byHand/housesSmart.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Reference\housemodel\data\T\byHand\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6ECDBD20-979C-4444-9C91-6E0B23E577B4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19DC5DD5-F49F-4A71-8E91-9A85EAD86ACE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="7200" yWindow="0" windowWidth="21600" windowHeight="15600" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -737,7 +737,21 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="116">
+  <dxfs count="118">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -2519,8 +2533,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0D0F27B-DE69-4889-8F79-7CACC7421700}">
   <dimension ref="A1:Y66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19:G26"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="Q19" sqref="Q19:Q26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3789,9 +3803,11 @@
       </c>
       <c r="K19" t="str">
         <f t="shared" si="7"/>
-        <v>Pending</v>
-      </c>
-      <c r="L19" s="7"/>
+        <v>Done</v>
+      </c>
+      <c r="L19" s="7">
+        <v>44025</v>
+      </c>
       <c r="M19" s="27" t="s">
         <v>16</v>
       </c>
@@ -3800,9 +3816,11 @@
       </c>
       <c r="P19" t="str">
         <f t="shared" si="8"/>
-        <v>Pending</v>
-      </c>
-      <c r="Q19" s="7"/>
+        <v>Done</v>
+      </c>
+      <c r="Q19" s="7">
+        <v>44025</v>
+      </c>
       <c r="R19" s="27" t="s">
         <v>16</v>
       </c>
@@ -3917,7 +3935,10 @@
       </c>
       <c r="K21" t="str">
         <f t="shared" si="7"/>
-        <v>Pending</v>
+        <v>Done</v>
+      </c>
+      <c r="L21" s="7">
+        <v>44025</v>
       </c>
       <c r="M21" s="27" t="s">
         <v>15</v>
@@ -3927,7 +3948,10 @@
       </c>
       <c r="P21" t="str">
         <f t="shared" si="8"/>
-        <v>Pending</v>
+        <v>Done</v>
+      </c>
+      <c r="Q21" s="7">
+        <v>44025</v>
       </c>
       <c r="R21" s="27" t="s">
         <v>15</v>
@@ -3975,7 +3999,10 @@
       </c>
       <c r="K22" t="str">
         <f t="shared" si="7"/>
-        <v>Pending</v>
+        <v>Done</v>
+      </c>
+      <c r="L22" s="7">
+        <v>44025</v>
       </c>
       <c r="M22" s="27" t="s">
         <v>6</v>
@@ -3985,7 +4012,10 @@
       </c>
       <c r="P22" t="str">
         <f t="shared" si="8"/>
-        <v>Pending</v>
+        <v>Done</v>
+      </c>
+      <c r="Q22" s="7">
+        <v>44025</v>
       </c>
       <c r="R22" s="27" t="s">
         <v>6</v>
@@ -4033,7 +4063,10 @@
       </c>
       <c r="K23" t="str">
         <f t="shared" si="7"/>
-        <v>Pending</v>
+        <v>Done</v>
+      </c>
+      <c r="L23" s="7">
+        <v>44025</v>
       </c>
       <c r="M23" s="27" t="s">
         <v>8</v>
@@ -4043,7 +4076,10 @@
       </c>
       <c r="P23" t="str">
         <f t="shared" si="8"/>
-        <v>Pending</v>
+        <v>Done</v>
+      </c>
+      <c r="Q23" s="7">
+        <v>44025</v>
       </c>
       <c r="R23" s="27" t="s">
         <v>8</v>
@@ -4091,7 +4127,10 @@
       </c>
       <c r="K24" t="str">
         <f t="shared" si="7"/>
-        <v>Pending</v>
+        <v>Done</v>
+      </c>
+      <c r="L24" s="7">
+        <v>44025</v>
       </c>
       <c r="M24" s="27" t="s">
         <v>9</v>
@@ -4101,7 +4140,10 @@
       </c>
       <c r="P24" t="str">
         <f t="shared" si="8"/>
-        <v>Pending</v>
+        <v>Done</v>
+      </c>
+      <c r="Q24" s="7">
+        <v>44025</v>
       </c>
       <c r="R24" s="27" t="s">
         <v>9</v>
@@ -4149,7 +4191,10 @@
       </c>
       <c r="K25" t="str">
         <f t="shared" si="7"/>
-        <v>Pending</v>
+        <v>Done</v>
+      </c>
+      <c r="L25" s="7">
+        <v>44025</v>
       </c>
       <c r="M25" s="27" t="s">
         <v>10</v>
@@ -4159,7 +4204,10 @@
       </c>
       <c r="P25" t="str">
         <f t="shared" si="8"/>
-        <v>Pending</v>
+        <v>Done</v>
+      </c>
+      <c r="Q25" s="7">
+        <v>44025</v>
       </c>
       <c r="R25" s="27" t="s">
         <v>10</v>
@@ -4207,9 +4255,11 @@
       </c>
       <c r="K26" t="str">
         <f>IF(ISBLANK(L26),"Pending","Done")</f>
-        <v>Pending</v>
-      </c>
-      <c r="L26" s="7"/>
+        <v>Done</v>
+      </c>
+      <c r="L26" s="7">
+        <v>44025</v>
+      </c>
       <c r="M26" s="27" t="s">
         <v>92</v>
       </c>
@@ -4218,9 +4268,11 @@
       </c>
       <c r="P26" t="str">
         <f>IF(ISBLANK(Q26),"Pending","Done")</f>
-        <v>Pending</v>
-      </c>
-      <c r="Q26" s="7"/>
+        <v>Done</v>
+      </c>
+      <c r="Q26" s="7">
+        <v>44025</v>
+      </c>
       <c r="R26" s="27" t="s">
         <v>92</v>
       </c>
@@ -6765,430 +6817,430 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A3:B13">
-    <cfRule type="cellIs" dxfId="115" priority="125" operator="equal">
+    <cfRule type="cellIs" dxfId="117" priority="129" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="114" priority="126" operator="equal">
+    <cfRule type="cellIs" dxfId="116" priority="130" operator="equal">
       <formula>"Done"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F3:G4 F6:G6 F5 F13:G13 F7:F12">
-    <cfRule type="cellIs" dxfId="113" priority="123" operator="equal">
+    <cfRule type="cellIs" dxfId="115" priority="127" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="112" priority="124" operator="equal">
+    <cfRule type="cellIs" dxfId="114" priority="128" operator="equal">
       <formula>"Done"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K3:L4 K6:L6 K5 K13:L13 K7:K12">
-    <cfRule type="cellIs" dxfId="111" priority="121" operator="equal">
+    <cfRule type="cellIs" dxfId="113" priority="125" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="110" priority="122" operator="equal">
+    <cfRule type="cellIs" dxfId="112" priority="126" operator="equal">
       <formula>"Done"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P3:Q4 P6:Q6 P5 P13:Q13 P7:P12">
-    <cfRule type="cellIs" dxfId="109" priority="119" operator="equal">
+    <cfRule type="cellIs" dxfId="111" priority="123" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="108" priority="120" operator="equal">
+    <cfRule type="cellIs" dxfId="110" priority="124" operator="equal">
       <formula>"Done"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U3:V4 U6:V6 U5 U13:V13 U7:U12">
-    <cfRule type="cellIs" dxfId="107" priority="117" operator="equal">
+    <cfRule type="cellIs" dxfId="109" priority="121" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="106" priority="118" operator="equal">
+    <cfRule type="cellIs" dxfId="108" priority="122" operator="equal">
       <formula>"Done"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A16:B27">
-    <cfRule type="cellIs" dxfId="105" priority="115" operator="equal">
+    <cfRule type="cellIs" dxfId="107" priority="119" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="104" priority="116" operator="equal">
+    <cfRule type="cellIs" dxfId="106" priority="120" operator="equal">
       <formula>"Done"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F16:F26">
-    <cfRule type="cellIs" dxfId="103" priority="113" operator="equal">
+    <cfRule type="cellIs" dxfId="105" priority="117" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="102" priority="114" operator="equal">
+    <cfRule type="cellIs" dxfId="104" priority="118" operator="equal">
       <formula>"Done"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K16:K26">
-    <cfRule type="cellIs" dxfId="101" priority="111" operator="equal">
+    <cfRule type="cellIs" dxfId="103" priority="115" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="100" priority="112" operator="equal">
+    <cfRule type="cellIs" dxfId="102" priority="116" operator="equal">
       <formula>"Done"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P16:P26">
-    <cfRule type="cellIs" dxfId="99" priority="109" operator="equal">
+    <cfRule type="cellIs" dxfId="101" priority="113" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="98" priority="110" operator="equal">
+    <cfRule type="cellIs" dxfId="100" priority="114" operator="equal">
       <formula>"Done"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U16:U26">
-    <cfRule type="cellIs" dxfId="97" priority="107" operator="equal">
+    <cfRule type="cellIs" dxfId="99" priority="111" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="96" priority="108" operator="equal">
+    <cfRule type="cellIs" dxfId="98" priority="112" operator="equal">
       <formula>"Done"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G5">
-    <cfRule type="cellIs" dxfId="95" priority="95" operator="equal">
+    <cfRule type="cellIs" dxfId="97" priority="99" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="94" priority="96" operator="equal">
+    <cfRule type="cellIs" dxfId="96" priority="100" operator="equal">
       <formula>"Done"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G7:G12">
-    <cfRule type="cellIs" dxfId="93" priority="93" operator="equal">
+    <cfRule type="cellIs" dxfId="95" priority="97" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="92" priority="94" operator="equal">
+    <cfRule type="cellIs" dxfId="94" priority="98" operator="equal">
       <formula>"Done"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L5">
-    <cfRule type="cellIs" dxfId="91" priority="91" operator="equal">
+    <cfRule type="cellIs" dxfId="93" priority="95" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="90" priority="92" operator="equal">
+    <cfRule type="cellIs" dxfId="92" priority="96" operator="equal">
       <formula>"Done"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L7:L12">
-    <cfRule type="cellIs" dxfId="89" priority="89" operator="equal">
+    <cfRule type="cellIs" dxfId="91" priority="93" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="88" priority="90" operator="equal">
+    <cfRule type="cellIs" dxfId="90" priority="94" operator="equal">
       <formula>"Done"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q5">
-    <cfRule type="cellIs" dxfId="87" priority="87" operator="equal">
+    <cfRule type="cellIs" dxfId="89" priority="91" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="86" priority="88" operator="equal">
+    <cfRule type="cellIs" dxfId="88" priority="92" operator="equal">
       <formula>"Done"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q7:Q12">
-    <cfRule type="cellIs" dxfId="85" priority="85" operator="equal">
+    <cfRule type="cellIs" dxfId="87" priority="89" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="84" priority="86" operator="equal">
+    <cfRule type="cellIs" dxfId="86" priority="90" operator="equal">
       <formula>"Done"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V5">
-    <cfRule type="cellIs" dxfId="83" priority="83" operator="equal">
+    <cfRule type="cellIs" dxfId="85" priority="87" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="82" priority="84" operator="equal">
+    <cfRule type="cellIs" dxfId="84" priority="88" operator="equal">
       <formula>"Done"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V7:V12">
-    <cfRule type="cellIs" dxfId="81" priority="81" operator="equal">
+    <cfRule type="cellIs" dxfId="83" priority="85" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="80" priority="82" operator="equal">
+    <cfRule type="cellIs" dxfId="82" priority="86" operator="equal">
       <formula>"Done"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A30:B40">
-    <cfRule type="cellIs" dxfId="79" priority="79" operator="equal">
+    <cfRule type="cellIs" dxfId="81" priority="83" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="78" priority="80" operator="equal">
+    <cfRule type="cellIs" dxfId="80" priority="84" operator="equal">
       <formula>"Done"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F30:F40">
-    <cfRule type="cellIs" dxfId="77" priority="77" operator="equal">
+    <cfRule type="cellIs" dxfId="79" priority="81" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="76" priority="78" operator="equal">
+    <cfRule type="cellIs" dxfId="78" priority="82" operator="equal">
       <formula>"Done"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K30:K40">
-    <cfRule type="cellIs" dxfId="75" priority="75" operator="equal">
+    <cfRule type="cellIs" dxfId="77" priority="79" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="74" priority="76" operator="equal">
+    <cfRule type="cellIs" dxfId="76" priority="80" operator="equal">
       <formula>"Done"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P30:P40">
-    <cfRule type="cellIs" dxfId="73" priority="73" operator="equal">
+    <cfRule type="cellIs" dxfId="75" priority="77" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="72" priority="74" operator="equal">
+    <cfRule type="cellIs" dxfId="74" priority="78" operator="equal">
       <formula>"Done"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U30:U40">
-    <cfRule type="cellIs" dxfId="71" priority="71" operator="equal">
+    <cfRule type="cellIs" dxfId="73" priority="75" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="70" priority="72" operator="equal">
+    <cfRule type="cellIs" dxfId="72" priority="76" operator="equal">
       <formula>"Done"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G30:G40">
-    <cfRule type="cellIs" dxfId="69" priority="69" operator="equal">
+    <cfRule type="cellIs" dxfId="71" priority="73" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="68" priority="70" operator="equal">
+    <cfRule type="cellIs" dxfId="70" priority="74" operator="equal">
       <formula>"Done"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L30:L40">
-    <cfRule type="cellIs" dxfId="67" priority="67" operator="equal">
+    <cfRule type="cellIs" dxfId="69" priority="71" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="66" priority="68" operator="equal">
+    <cfRule type="cellIs" dxfId="68" priority="72" operator="equal">
       <formula>"Done"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q30:Q40">
-    <cfRule type="cellIs" dxfId="65" priority="65" operator="equal">
+    <cfRule type="cellIs" dxfId="67" priority="69" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="64" priority="66" operator="equal">
+    <cfRule type="cellIs" dxfId="66" priority="70" operator="equal">
       <formula>"Done"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V30:V40">
-    <cfRule type="cellIs" dxfId="63" priority="63" operator="equal">
+    <cfRule type="cellIs" dxfId="65" priority="67" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="62" priority="64" operator="equal">
+    <cfRule type="cellIs" dxfId="64" priority="68" operator="equal">
       <formula>"Done"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A43:B53">
-    <cfRule type="cellIs" dxfId="61" priority="61" operator="equal">
+    <cfRule type="cellIs" dxfId="63" priority="65" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="60" priority="62" operator="equal">
+    <cfRule type="cellIs" dxfId="62" priority="66" operator="equal">
       <formula>"Done"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F43:F53">
-    <cfRule type="cellIs" dxfId="59" priority="59" operator="equal">
+    <cfRule type="cellIs" dxfId="61" priority="63" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="58" priority="60" operator="equal">
+    <cfRule type="cellIs" dxfId="60" priority="64" operator="equal">
       <formula>"Done"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K43:K53">
-    <cfRule type="cellIs" dxfId="57" priority="57" operator="equal">
+    <cfRule type="cellIs" dxfId="59" priority="61" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="56" priority="58" operator="equal">
+    <cfRule type="cellIs" dxfId="58" priority="62" operator="equal">
       <formula>"Done"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P43:P53">
-    <cfRule type="cellIs" dxfId="55" priority="55" operator="equal">
+    <cfRule type="cellIs" dxfId="57" priority="59" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="54" priority="56" operator="equal">
+    <cfRule type="cellIs" dxfId="56" priority="60" operator="equal">
       <formula>"Done"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U43:U53">
-    <cfRule type="cellIs" dxfId="53" priority="53" operator="equal">
+    <cfRule type="cellIs" dxfId="55" priority="57" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="52" priority="54" operator="equal">
+    <cfRule type="cellIs" dxfId="54" priority="58" operator="equal">
       <formula>"Done"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G43:G53">
-    <cfRule type="cellIs" dxfId="51" priority="51" operator="equal">
+    <cfRule type="cellIs" dxfId="53" priority="55" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="50" priority="52" operator="equal">
+    <cfRule type="cellIs" dxfId="52" priority="56" operator="equal">
       <formula>"Done"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L43:L53">
-    <cfRule type="cellIs" dxfId="49" priority="49" operator="equal">
+    <cfRule type="cellIs" dxfId="51" priority="53" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="48" priority="50" operator="equal">
+    <cfRule type="cellIs" dxfId="50" priority="54" operator="equal">
       <formula>"Done"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q43:Q53">
-    <cfRule type="cellIs" dxfId="47" priority="47" operator="equal">
+    <cfRule type="cellIs" dxfId="49" priority="51" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="46" priority="48" operator="equal">
+    <cfRule type="cellIs" dxfId="48" priority="52" operator="equal">
       <formula>"Done"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V43:V53">
-    <cfRule type="cellIs" dxfId="45" priority="45" operator="equal">
+    <cfRule type="cellIs" dxfId="47" priority="49" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="44" priority="46" operator="equal">
+    <cfRule type="cellIs" dxfId="46" priority="50" operator="equal">
       <formula>"Done"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A56:B66">
-    <cfRule type="cellIs" dxfId="43" priority="43" operator="equal">
+    <cfRule type="cellIs" dxfId="45" priority="47" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="42" priority="44" operator="equal">
+    <cfRule type="cellIs" dxfId="44" priority="48" operator="equal">
       <formula>"Done"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F56:F66">
-    <cfRule type="cellIs" dxfId="41" priority="41" operator="equal">
+    <cfRule type="cellIs" dxfId="43" priority="45" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="40" priority="42" operator="equal">
+    <cfRule type="cellIs" dxfId="42" priority="46" operator="equal">
       <formula>"Done"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K56:K66">
-    <cfRule type="cellIs" dxfId="39" priority="39" operator="equal">
+    <cfRule type="cellIs" dxfId="41" priority="43" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="38" priority="40" operator="equal">
+    <cfRule type="cellIs" dxfId="40" priority="44" operator="equal">
       <formula>"Done"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P56:P66">
-    <cfRule type="cellIs" dxfId="37" priority="37" operator="equal">
+    <cfRule type="cellIs" dxfId="39" priority="41" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="36" priority="38" operator="equal">
+    <cfRule type="cellIs" dxfId="38" priority="42" operator="equal">
       <formula>"Done"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U56:U66">
-    <cfRule type="cellIs" dxfId="35" priority="35" operator="equal">
+    <cfRule type="cellIs" dxfId="37" priority="39" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="34" priority="36" operator="equal">
+    <cfRule type="cellIs" dxfId="36" priority="40" operator="equal">
       <formula>"Done"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G56:G66">
-    <cfRule type="cellIs" dxfId="33" priority="33" operator="equal">
+    <cfRule type="cellIs" dxfId="35" priority="37" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="32" priority="34" operator="equal">
+    <cfRule type="cellIs" dxfId="34" priority="38" operator="equal">
       <formula>"Done"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L56:L66">
-    <cfRule type="cellIs" dxfId="31" priority="31" operator="equal">
+    <cfRule type="cellIs" dxfId="33" priority="35" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="30" priority="32" operator="equal">
+    <cfRule type="cellIs" dxfId="32" priority="36" operator="equal">
       <formula>"Done"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q56:Q66">
-    <cfRule type="cellIs" dxfId="29" priority="29" operator="equal">
+    <cfRule type="cellIs" dxfId="31" priority="33" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="28" priority="30" operator="equal">
+    <cfRule type="cellIs" dxfId="30" priority="34" operator="equal">
       <formula>"Done"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V56:V66">
-    <cfRule type="cellIs" dxfId="27" priority="27" operator="equal">
+    <cfRule type="cellIs" dxfId="29" priority="31" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="26" priority="28" operator="equal">
+    <cfRule type="cellIs" dxfId="28" priority="32" operator="equal">
       <formula>"Done"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F27">
-    <cfRule type="cellIs" dxfId="25" priority="25" operator="equal">
+    <cfRule type="cellIs" dxfId="27" priority="29" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="24" priority="26" operator="equal">
+    <cfRule type="cellIs" dxfId="26" priority="30" operator="equal">
       <formula>"Done"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K27">
-    <cfRule type="cellIs" dxfId="23" priority="23" operator="equal">
+    <cfRule type="cellIs" dxfId="25" priority="27" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="22" priority="24" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="28" operator="equal">
       <formula>"Done"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P27">
-    <cfRule type="cellIs" dxfId="21" priority="21" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="25" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="20" priority="22" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="26" operator="equal">
       <formula>"Done"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U27">
-    <cfRule type="cellIs" dxfId="19" priority="19" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="23" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="20" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="24" operator="equal">
       <formula>"Done"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G16:G18 G27">
-    <cfRule type="cellIs" dxfId="17" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="21" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="22" operator="equal">
       <formula>"Done"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L16:L19 L21:L27">
-    <cfRule type="cellIs" dxfId="15" priority="15" operator="equal">
+  <conditionalFormatting sqref="L16:L18 L27">
+    <cfRule type="cellIs" dxfId="17" priority="19" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="20" operator="equal">
       <formula>"Done"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Q16:Q19 Q21:Q27">
-    <cfRule type="cellIs" dxfId="13" priority="13" operator="equal">
+  <conditionalFormatting sqref="Q16:Q18 Q27">
+    <cfRule type="cellIs" dxfId="15" priority="17" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="18" operator="equal">
       <formula>"Done"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V16:V19 V21:V27">
-    <cfRule type="cellIs" dxfId="11" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="15" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="16" operator="equal">
       <formula>"Done"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L20">
+  <conditionalFormatting sqref="V20">
     <cfRule type="cellIs" dxfId="7" priority="7" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
@@ -7196,7 +7248,7 @@
       <formula>"Done"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Q20">
+  <conditionalFormatting sqref="G19:G26">
     <cfRule type="cellIs" dxfId="5" priority="5" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
@@ -7204,7 +7256,7 @@
       <formula>"Done"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="V20">
+  <conditionalFormatting sqref="L19:L26">
     <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
@@ -7212,7 +7264,7 @@
       <formula>"Done"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G19:G26">
+  <conditionalFormatting sqref="Q19:Q26">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>

</xml_diff>